<commit_message>
Generates .json file from excell table
</commit_message>
<xml_diff>
--- a/lib/md-to-json/src/test/resources/AIO_Daten_Arbeitsmappe.xlsx
+++ b/lib/md-to-json/src/test/resources/AIO_Daten_Arbeitsmappe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSO\OneDrive - OPITZ CONSULTING Deutschland GmbH\Daimler\Daten-und-praesie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{1DE88293-BAD2-4A33-AE89-BEC273F65B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D92CA576-3163-4878-9E8D-65C66C157968}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{1DE88293-BAD2-4A33-AE89-BEC273F65B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8C75D547-0FF0-46AA-97F5-EF8736097A11}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprachen" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="91">
   <si>
     <t>Java</t>
   </si>
@@ -682,9 +682,6 @@
   </si>
   <si>
     <t>Betriebswitschaftlich</t>
-  </si>
-  <si>
-    <t>Betriebswirtschaftlich</t>
   </si>
   <si>
     <t>RAM</t>
@@ -1761,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -2188,92 +2185,6 @@
       <c r="K30">
         <f>SUM(G30:I30)</f>
         <v>73.324675324675326</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="B76" t="s">
-        <v>63</v>
-      </c>
-      <c r="C76" t="s">
-        <v>64</v>
-      </c>
-      <c r="D76" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="str">
-        <f>Sprachen!A1</f>
-        <v>Java</v>
-      </c>
-      <c r="B77">
-        <v>80</v>
-      </c>
-      <c r="C77">
-        <v>100</v>
-      </c>
-      <c r="D77">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="str">
-        <f>Sprachen!A2</f>
-        <v>Go</v>
-      </c>
-      <c r="B78">
-        <v>100</v>
-      </c>
-      <c r="C78">
-        <v>100</v>
-      </c>
-      <c r="D78">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" t="str">
-        <f>Sprachen!A3</f>
-        <v>Rust</v>
-      </c>
-      <c r="B79">
-        <v>100</v>
-      </c>
-      <c r="C79">
-        <v>100</v>
-      </c>
-      <c r="D79">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" t="str">
-        <f>Sprachen!A4</f>
-        <v>C++</v>
-      </c>
-      <c r="B80">
-        <v>100</v>
-      </c>
-      <c r="C80">
-        <v>60</v>
-      </c>
-      <c r="D80">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="str">
-        <f>Sprachen!A5</f>
-        <v>Python</v>
-      </c>
-      <c r="B81">
-        <v>50</v>
-      </c>
-      <c r="C81">
-        <v>80</v>
-      </c>
-      <c r="D81">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2300,7 +2211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -2315,16 +2226,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>70</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -2895,22 +2806,22 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
         <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
       </c>
       <c r="E1" t="s">
         <v>55</v>
       </c>
       <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>74</v>
-      </c>
-      <c r="H1" t="s">
-        <v>75</v>
       </c>
       <c r="I1" t="s">
         <v>49</v>
@@ -4149,13 +4060,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>78</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -4576,8 +4487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -4591,22 +4502,22 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" t="s">
-        <v>84</v>
       </c>
       <c r="J1" t="s">
         <v>13</v>
@@ -5480,13 +5391,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>86</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -5912,16 +5823,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -7559,7 +7470,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>

</xml_diff>